<commit_message>
Case Blankenge with density added.
</commit_message>
<xml_diff>
--- a/Projects/Density/cases/RotatingIface/RotatingIface.xlsx
+++ b/Projects/Density/cases/RotatingIface/RotatingIface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Density/cases/RotatingIface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39836110-CFF8-F148-9BB5-155877CBE837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F355861-59F0-DF4F-8AE4-2D6EE5448620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="-23740" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11882,7 +11882,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13662,7 +13662,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <f>B5*tsmult</f>
+        <f t="shared" ref="B6:B18" si="0">B5*tsmult</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -13678,7 +13678,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <f>B6*tsmult</f>
+        <f t="shared" si="0"/>
         <v>1.2100000000000002</v>
       </c>
       <c r="F7">
@@ -13691,7 +13691,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <f>B7*tsmult</f>
+        <f t="shared" si="0"/>
         <v>1.3310000000000004</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -13706,7 +13706,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <f>B8*tsmult</f>
+        <f t="shared" si="0"/>
         <v>1.4641000000000006</v>
       </c>
     </row>
@@ -13715,7 +13715,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <f>B9*tsmult</f>
+        <f t="shared" si="0"/>
         <v>1.6105100000000008</v>
       </c>
     </row>
@@ -13724,7 +13724,7 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <f>B10*tsmult</f>
+        <f t="shared" si="0"/>
         <v>1.7715610000000011</v>
       </c>
     </row>
@@ -13733,7 +13733,7 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <f>B11*tsmult</f>
+        <f t="shared" si="0"/>
         <v>1.9487171000000014</v>
       </c>
     </row>
@@ -13742,7 +13742,7 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <f>B12*tsmult</f>
+        <f t="shared" si="0"/>
         <v>2.1435888100000016</v>
       </c>
     </row>
@@ -13751,7 +13751,7 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <f>B13*tsmult</f>
+        <f t="shared" si="0"/>
         <v>2.3579476910000019</v>
       </c>
     </row>
@@ -13760,7 +13760,7 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <f>B14*tsmult</f>
+        <f t="shared" si="0"/>
         <v>2.5937424601000023</v>
       </c>
     </row>
@@ -13769,7 +13769,7 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <f>B15*tsmult</f>
+        <f t="shared" si="0"/>
         <v>2.8531167061100029</v>
       </c>
     </row>
@@ -13778,7 +13778,7 @@
         <v>12</v>
       </c>
       <c r="B17">
-        <f>B16*tsmult</f>
+        <f t="shared" si="0"/>
         <v>3.1384283767210035</v>
       </c>
     </row>
@@ -13787,7 +13787,7 @@
         <v>13</v>
       </c>
       <c r="B18">
-        <f>B17*tsmult</f>
+        <f t="shared" si="0"/>
         <v>3.4522712143931042</v>
       </c>
     </row>

</xml_diff>